<commit_message>
Javadoc, complexity, some optimization
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
@@ -154,13 +154,367 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$F$4:$J$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$H$4:$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$F$5:$J$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$H$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>389</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4465</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10240</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C3EC-40D9-AC69-3E8F168E874D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$F$4:$J$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$H$4:$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$F$6:$J$6</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$H$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1206</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8553</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23697</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C3EC-40D9-AC69-3E8F168E874D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$F$4:$J$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$H$4:$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$F$7:$J$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$H$7:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1850</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13461</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34877</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C3EC-40D9-AC69-3E8F168E874D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$F$4:$J$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$H$4:$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$F$8:$J$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$H$8:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2152</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13594</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32859</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C3EC-40D9-AC69-3E8F168E874D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="384781808"/>
+        <c:axId val="384783448"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="384781808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -172,17 +526,163 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:r>
-              <a:rPr lang="nl-NL"/>
-              <a:t>Execution</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="nl-NL" baseline="0"/>
-              <a:t> Seed</a:t>
-            </a:r>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
-        </c:rich>
-      </c:tx>
+        </c:txPr>
+        <c:crossAx val="384783448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="384783448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="384781808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -236,50 +736,12 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="7"/>
-              <c:pt idx="0">
-                <c:v>1</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>3</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>4</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>5</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>6</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>8</c:v>
-              </c:pt>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:autoCat val="1"/>
-                </c:ext>
-              </c:extLst>
-            </c:strLit>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Sheet1!$C$5:$J$5</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(Sheet1!$C$5:$H$5,Sheet1!$J$5)</c:f>
+              <c:f>Sheet1!$C$5:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -299,6 +761,9 @@
                   <c:v>389</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>4465</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>10240</c:v>
                 </c:pt>
               </c:numCache>
@@ -307,7 +772,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BF23-4E96-A7A8-867789E464EE}"/>
+              <c16:uniqueId val="{00000000-E882-4AB3-B052-99425632AF41}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -329,50 +794,12 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="7"/>
-              <c:pt idx="0">
-                <c:v>1</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>3</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>4</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>5</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>6</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>8</c:v>
-              </c:pt>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:autoCat val="1"/>
-                </c:ext>
-              </c:extLst>
-            </c:strLit>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Sheet1!$C$6:$J$6</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(Sheet1!$C$6:$H$6,Sheet1!$J$6)</c:f>
+              <c:f>Sheet1!$C$6:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -380,19 +807,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>122</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2044</c:v>
+                  <c:v>1206</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33930</c:v>
+                  <c:v>8553</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23697</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -400,7 +830,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-BF23-4E96-A7A8-867789E464EE}"/>
+              <c16:uniqueId val="{00000001-E882-4AB3-B052-99425632AF41}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -408,7 +838,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>concordance</c:v>
+            <c:v>Concordance</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -422,50 +852,12 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="7"/>
-              <c:pt idx="0">
-                <c:v>1</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>3</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>4</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>5</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>6</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>8</c:v>
-              </c:pt>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:autoCat val="1"/>
-                </c:ext>
-              </c:extLst>
-            </c:strLit>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Sheet1!$C$7:$J$7</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(Sheet1!$C$7:$H$7,Sheet1!$J$7)</c:f>
+              <c:f>Sheet1!$C$7:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -473,19 +865,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>122</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1850</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38113</c:v>
+                  <c:v>13461</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34877</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -493,7 +888,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-BF23-4E96-A7A8-867789E464EE}"/>
+              <c16:uniqueId val="{00000002-E882-4AB3-B052-99425632AF41}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -501,7 +896,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>frequence</c:v>
+            <c:v>Frequence</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -515,70 +910,35 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="7"/>
-              <c:pt idx="0">
-                <c:v>1</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>3</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>4</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>5</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>6</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>8</c:v>
-              </c:pt>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:autoCat val="1"/>
-                </c:ext>
-              </c:extLst>
-            </c:strLit>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Sheet1!$C$8:$J$8</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(Sheet1!$C$8:$H$8,Sheet1!$J$8)</c:f>
+              <c:f>Sheet1!$C$8:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>163</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2561</c:v>
+                  <c:v>2152</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39808</c:v>
+                  <c:v>13594</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32859</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -586,7 +946,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-BF23-4E96-A7A8-867789E464EE}"/>
+              <c16:uniqueId val="{00000003-E882-4AB3-B052-99425632AF41}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -599,17 +959,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="487638224"/>
-        <c:axId val="487630352"/>
+        <c:axId val="476531360"/>
+        <c:axId val="476531688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="487638224"/>
+        <c:axId val="476531360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -645,14 +1005,15 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="487630352"/>
+        <c:crossAx val="476531688"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="487630352"/>
+        <c:axId val="476531688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -673,7 +1034,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -703,7 +1064,8 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="487638224"/>
+        <c:crossAx val="476531360"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -822,8 +1184,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -931,6 +1333,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -941,6 +1348,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -972,6 +1384,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1027,23 +1442,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1213,17 +1627,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1292,20 +1695,535 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1342,23 +2260,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96BB3673-AF2B-4310-90CE-9628F499766D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59473EF6-98B0-41DC-963D-6BBCBA44C1FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1371,6 +2289,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF7DAB6B-A42A-4F0B-93E5-09AD76763E93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1662,8 +2616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1677,6 +2631,7 @@
     <col min="8" max="8" width="10.44140625" customWidth="1"/>
     <col min="9" max="9" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
@@ -1757,7 +2712,7 @@
         <v>389</v>
       </c>
       <c r="I5">
-        <v>416</v>
+        <v>4465</v>
       </c>
       <c r="J5">
         <v>10240</v>
@@ -1774,22 +2729,22 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G6">
-        <v>122</v>
+        <v>66</v>
       </c>
       <c r="H6">
-        <v>2044</v>
+        <v>1206</v>
       </c>
       <c r="I6">
-        <v>14101</v>
+        <v>8553</v>
       </c>
       <c r="J6">
-        <v>33930</v>
+        <v>23697</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
@@ -1803,22 +2758,22 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="H7">
         <v>1850</v>
       </c>
       <c r="I7">
-        <v>14353</v>
+        <v>13461</v>
       </c>
       <c r="J7">
-        <v>38113</v>
+        <v>34877</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
@@ -1826,28 +2781,28 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F8">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="H8">
-        <v>2561</v>
+        <v>2152</v>
       </c>
       <c r="I8">
-        <v>16162</v>
+        <v>13594</v>
       </c>
       <c r="J8">
-        <v>39808</v>
+        <v>32859</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added alice in wonderland book + tets
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
@@ -1720,7 +1720,7 @@
   <dimension ref="B3:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>